<commit_message>
Adder page added in excel
</commit_message>
<xml_diff>
--- a/useful references/Hex_Decimal_Binary Conversion & Truth Tables.xlsx
+++ b/useful references/Hex_Decimal_Binary Conversion & Truth Tables.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\Specifications\ATE Test Equipment\Harrison Warke\Verilog_HDLBits\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\Specifications\ATE Test Equipment\Harrison Warke\Verilog_HDLBits\useful references\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F174E8CD-6D1C-4505-A3DA-7DE70480C018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC7B9917-4A6C-44ED-B994-9DD85CE6431B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13800" yWindow="-16308" windowWidth="29016" windowHeight="15696" activeTab="1" xr2:uid="{9E27DF17-1687-49C3-9253-CE9DE59247CA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{9E27DF17-1687-49C3-9253-CE9DE59247CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Hex_Dec_Bin Conversions" sheetId="1" r:id="rId1"/>
     <sheet name="Truth Tables" sheetId="3" r:id="rId2"/>
-    <sheet name="Bitwise Operators " sheetId="4" r:id="rId3"/>
+    <sheet name="Adders" sheetId="5" r:id="rId3"/>
+    <sheet name="Bitwise Operators " sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="42">
   <si>
     <t>HEX</t>
   </si>
@@ -110,13 +111,67 @@
   </si>
   <si>
     <t>Cout</t>
+  </si>
+  <si>
+    <t>inputs</t>
+  </si>
+  <si>
+    <t>outputs</t>
+  </si>
+  <si>
+    <t>Binary Addition Rules</t>
+  </si>
+  <si>
+    <t>0 + 0 = 0</t>
+  </si>
+  <si>
+    <t>a)</t>
+  </si>
+  <si>
+    <t>0 + 1 = 1</t>
+  </si>
+  <si>
+    <t>1 + 1 = 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 + 0 = 1 </t>
+  </si>
+  <si>
+    <t>c)</t>
+  </si>
+  <si>
+    <t>d)</t>
+  </si>
+  <si>
+    <t>b)</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>1 + 1 + 1 = 11</t>
+  </si>
+  <si>
+    <t>e)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sum </t>
+  </si>
+  <si>
+    <t>Half Adder</t>
+  </si>
+  <si>
+    <t>Example</t>
+  </si>
+  <si>
+    <t>The carry in comes from the previous stage of a mult-bit adder</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,6 +181,19 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -145,7 +213,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -313,11 +381,111 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -423,6 +591,145 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -854,48 +1161,67 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E26DB1B-1D8A-4D26-987D-BF5334090922}">
-  <dimension ref="B1:R18"/>
+  <dimension ref="A1:R18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="S9" sqref="S9"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2:R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="s">
+    <row r="1" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="28"/>
-      <c r="F2" s="26" t="s">
+      <c r="C2" s="38"/>
+      <c r="D2" s="39"/>
+      <c r="F2" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="27"/>
-      <c r="H2" s="28"/>
-      <c r="J2" s="26" t="s">
+      <c r="G2" s="38"/>
+      <c r="H2" s="39"/>
+      <c r="J2" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="27"/>
-      <c r="L2" s="28"/>
-      <c r="N2" s="26" t="s">
+      <c r="K2" s="38"/>
+      <c r="L2" s="39"/>
+      <c r="N2" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="O2" s="27"/>
-      <c r="P2" s="27"/>
-      <c r="Q2" s="27"/>
-      <c r="R2" s="28"/>
-    </row>
-    <row r="3" spans="2:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="2:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O2" s="38"/>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="38"/>
+      <c r="R2" s="39"/>
+    </row>
+    <row r="3" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="41"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="41"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="46"/>
+      <c r="J3" s="52"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="43"/>
+      <c r="M3" s="41"/>
+      <c r="O3" s="49" t="s">
+        <v>24</v>
+      </c>
+      <c r="P3" s="42"/>
+      <c r="Q3" s="50" t="s">
+        <v>25</v>
+      </c>
+      <c r="R3" s="51"/>
+    </row>
+    <row r="4" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="48" t="s">
         <v>8</v>
       </c>
       <c r="F4" s="16" t="s">
@@ -932,7 +1258,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B5" s="15">
         <v>0</v>
       </c>
@@ -976,7 +1302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B6" s="15">
         <v>0</v>
       </c>
@@ -1020,7 +1346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B7" s="15">
         <v>1</v>
       </c>
@@ -1064,7 +1390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="13">
         <v>1</v>
       </c>
@@ -1108,7 +1434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B9" s="19"/>
       <c r="C9" s="19"/>
       <c r="D9" s="19"/>
@@ -1133,7 +1459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="N10" s="18">
         <v>1</v>
       </c>
@@ -1150,7 +1476,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="N11" s="18">
         <v>1</v>
       </c>
@@ -1167,22 +1493,22 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="26" t="s">
+    <row r="12" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="27"/>
-      <c r="D12" s="28"/>
-      <c r="F12" s="26" t="s">
+      <c r="C12" s="38"/>
+      <c r="D12" s="39"/>
+      <c r="F12" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="27"/>
-      <c r="H12" s="28"/>
-      <c r="J12" s="26" t="s">
+      <c r="G12" s="38"/>
+      <c r="H12" s="39"/>
+      <c r="J12" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="K12" s="27"/>
-      <c r="L12" s="28"/>
+      <c r="K12" s="38"/>
+      <c r="L12" s="39"/>
       <c r="N12" s="1">
         <v>1</v>
       </c>
@@ -1199,8 +1525,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="2:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="41"/>
+      <c r="C13" s="42"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="41"/>
+      <c r="G13" s="42"/>
+      <c r="H13" s="44"/>
+      <c r="I13" s="41"/>
+      <c r="K13" s="42"/>
+      <c r="L13" s="42"/>
+    </row>
+    <row r="14" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="16" t="s">
         <v>6</v>
       </c>
@@ -1216,7 +1552,7 @@
       <c r="G14" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="H14" s="9" t="s">
+      <c r="H14" s="45" t="s">
         <v>8</v>
       </c>
       <c r="J14" s="16" t="s">
@@ -1229,7 +1565,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B15" s="15">
         <v>0</v>
       </c>
@@ -1258,7 +1594,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B16" s="15">
         <v>0</v>
       </c>
@@ -1346,7 +1682,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="9">
     <mergeCell ref="N2:R2"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="F2:H2"/>
@@ -1354,12 +1690,769 @@
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="F12:H12"/>
     <mergeCell ref="J12:L12"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="J3:K3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{213E918A-C30F-4CEB-8DA0-5180A40C8188}">
+  <dimension ref="A2:U31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V21" sqref="V21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="9" max="9" width="13.59765625" customWidth="1"/>
+    <col min="10" max="10" width="11.19921875" customWidth="1"/>
+    <col min="11" max="11" width="11.296875" customWidth="1"/>
+    <col min="13" max="22" width="3.8984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:21" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="63"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+    </row>
+    <row r="3" spans="1:21" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="63"/>
+      <c r="B3" s="77" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="78"/>
+      <c r="D3" s="78"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="77" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="88"/>
+      <c r="J3" s="60"/>
+      <c r="K3" s="60"/>
+      <c r="L3" s="77" t="s">
+        <v>40</v>
+      </c>
+      <c r="M3" s="89"/>
+      <c r="N3" s="89"/>
+      <c r="O3" s="89"/>
+      <c r="P3" s="89"/>
+      <c r="Q3" s="89"/>
+      <c r="R3" s="89"/>
+      <c r="S3" s="89"/>
+      <c r="T3" s="88"/>
+    </row>
+    <row r="4" spans="1:21" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="63"/>
+      <c r="B4" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="54"/>
+      <c r="D4" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="54"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="63"/>
+      <c r="H4" s="81"/>
+      <c r="I4" s="82"/>
+    </row>
+    <row r="5" spans="1:21" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="63"/>
+      <c r="B5" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="56"/>
+      <c r="G5" s="63"/>
+      <c r="H5" s="55" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" s="83" t="s">
+        <v>27</v>
+      </c>
+      <c r="J5" s="59"/>
+      <c r="K5" s="59"/>
+      <c r="L5" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q5" s="57">
+        <v>1</v>
+      </c>
+      <c r="R5" s="57">
+        <v>1</v>
+      </c>
+      <c r="S5" s="57">
+        <v>0</v>
+      </c>
+      <c r="T5" s="57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" s="63"/>
+      <c r="B6" s="18">
+        <v>0</v>
+      </c>
+      <c r="C6" s="15">
+        <v>0</v>
+      </c>
+      <c r="D6" s="15">
+        <v>0</v>
+      </c>
+      <c r="E6" s="30">
+        <v>0</v>
+      </c>
+      <c r="F6" s="67"/>
+      <c r="G6" s="65"/>
+      <c r="H6" s="84" t="s">
+        <v>34</v>
+      </c>
+      <c r="I6" s="85" t="s">
+        <v>29</v>
+      </c>
+      <c r="J6" s="58"/>
+      <c r="K6" s="58"/>
+      <c r="L6" t="s">
+        <v>7</v>
+      </c>
+      <c r="N6" s="57"/>
+      <c r="O6" s="57"/>
+      <c r="P6" s="57"/>
+      <c r="Q6" s="57">
+        <v>1</v>
+      </c>
+      <c r="R6" s="57">
+        <v>0</v>
+      </c>
+      <c r="S6" s="57">
+        <v>1</v>
+      </c>
+      <c r="T6" s="57">
+        <v>0</v>
+      </c>
+      <c r="U6" s="71"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" s="63"/>
+      <c r="B7" s="29">
+        <v>0</v>
+      </c>
+      <c r="C7" s="21">
+        <v>1</v>
+      </c>
+      <c r="D7" s="17">
+        <v>1</v>
+      </c>
+      <c r="E7" s="30">
+        <v>0</v>
+      </c>
+      <c r="F7" s="67"/>
+      <c r="G7" s="65"/>
+      <c r="H7" s="84" t="s">
+        <v>32</v>
+      </c>
+      <c r="I7" s="86" t="s">
+        <v>31</v>
+      </c>
+      <c r="J7" s="49"/>
+      <c r="K7" s="49"/>
+      <c r="L7" s="74" t="s">
+        <v>35</v>
+      </c>
+      <c r="N7" s="57"/>
+      <c r="O7" s="57"/>
+      <c r="P7" s="57"/>
+      <c r="Q7" s="57"/>
+      <c r="R7" s="57"/>
+      <c r="S7" s="57"/>
+      <c r="T7" s="57"/>
+      <c r="U7" s="71"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="63"/>
+      <c r="B8" s="29">
+        <v>1</v>
+      </c>
+      <c r="C8" s="21">
+        <v>0</v>
+      </c>
+      <c r="D8" s="17">
+        <v>1</v>
+      </c>
+      <c r="E8" s="30">
+        <v>0</v>
+      </c>
+      <c r="F8" s="67"/>
+      <c r="G8" s="65"/>
+      <c r="H8" s="84" t="s">
+        <v>33</v>
+      </c>
+      <c r="I8" s="86" t="s">
+        <v>30</v>
+      </c>
+      <c r="J8" s="49"/>
+      <c r="K8" s="49"/>
+      <c r="L8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M8" s="66"/>
+      <c r="N8" s="70"/>
+      <c r="O8" s="70"/>
+      <c r="P8" s="70"/>
+      <c r="Q8" s="70">
+        <v>0</v>
+      </c>
+      <c r="R8" s="70">
+        <v>1</v>
+      </c>
+      <c r="S8" s="70">
+        <v>1</v>
+      </c>
+      <c r="T8" s="70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="63"/>
+      <c r="B9" s="1">
+        <v>1</v>
+      </c>
+      <c r="C9" s="13">
+        <v>1</v>
+      </c>
+      <c r="D9" s="13">
+        <v>0</v>
+      </c>
+      <c r="E9" s="36">
+        <v>1</v>
+      </c>
+      <c r="F9" s="67"/>
+      <c r="G9" s="65"/>
+      <c r="H9" s="87" t="s">
+        <v>37</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J9" s="49"/>
+      <c r="L9" s="61" t="s">
+        <v>23</v>
+      </c>
+      <c r="M9" s="75"/>
+      <c r="N9" s="76"/>
+      <c r="O9" s="73"/>
+      <c r="P9" s="95">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="95">
+        <v>0</v>
+      </c>
+      <c r="R9" s="95">
+        <v>0</v>
+      </c>
+      <c r="S9" s="95">
+        <v>0</v>
+      </c>
+      <c r="T9" s="73"/>
+      <c r="U9" s="63"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" s="63"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="67"/>
+      <c r="F10" s="67"/>
+      <c r="G10" s="65"/>
+      <c r="H10" s="63"/>
+      <c r="I10" s="63"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="72"/>
+      <c r="O10" s="72"/>
+      <c r="P10" s="72"/>
+      <c r="Q10" s="72"/>
+      <c r="R10" s="72"/>
+      <c r="S10" s="72"/>
+      <c r="T10" s="72"/>
+      <c r="U10" s="63"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" s="63"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="67"/>
+      <c r="F11" s="67"/>
+      <c r="G11" s="65"/>
+      <c r="H11" s="63"/>
+      <c r="I11" s="63"/>
+      <c r="M11" s="73"/>
+      <c r="N11" s="73"/>
+      <c r="O11" s="73"/>
+      <c r="P11" s="73"/>
+      <c r="Q11" s="73"/>
+      <c r="R11" s="73"/>
+      <c r="S11" s="69"/>
+      <c r="T11" s="73"/>
+      <c r="U11" s="63"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" s="63"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="67"/>
+      <c r="F12" s="67"/>
+      <c r="G12" s="65"/>
+      <c r="H12" s="63"/>
+      <c r="I12" s="63"/>
+      <c r="M12" s="63"/>
+      <c r="N12" s="63"/>
+      <c r="O12" s="63"/>
+      <c r="P12" s="63"/>
+      <c r="Q12" s="63"/>
+      <c r="R12" s="63"/>
+      <c r="S12" s="63"/>
+      <c r="T12" s="63"/>
+      <c r="U12" s="63"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" s="63"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="67"/>
+      <c r="F13" s="67"/>
+      <c r="G13" s="65"/>
+      <c r="H13" s="63"/>
+      <c r="I13" s="63"/>
+      <c r="M13" s="63"/>
+      <c r="N13" s="63"/>
+      <c r="O13" s="63"/>
+      <c r="P13" s="63"/>
+      <c r="Q13" s="63"/>
+      <c r="R13" s="63"/>
+      <c r="S13" s="63"/>
+      <c r="T13" s="63"/>
+      <c r="U13" s="63"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" s="63"/>
+      <c r="B14" s="63"/>
+      <c r="C14" s="63"/>
+      <c r="D14" s="63"/>
+      <c r="E14" s="65"/>
+      <c r="F14" s="65"/>
+      <c r="G14" s="65"/>
+      <c r="H14" s="63"/>
+      <c r="I14" s="63"/>
+      <c r="M14" s="63"/>
+      <c r="N14" s="63"/>
+      <c r="O14" s="63"/>
+      <c r="P14" s="63"/>
+      <c r="Q14" s="63"/>
+      <c r="R14" s="63"/>
+      <c r="S14" s="63"/>
+      <c r="T14" s="63"/>
+      <c r="U14" s="63"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" s="63"/>
+      <c r="B15" s="63"/>
+      <c r="C15" s="63"/>
+      <c r="D15" s="63"/>
+      <c r="E15" s="63"/>
+      <c r="F15" s="63"/>
+      <c r="G15" s="63"/>
+      <c r="H15" s="63"/>
+      <c r="I15" s="63"/>
+    </row>
+    <row r="20" spans="2:21" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="2:21" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="77" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="89"/>
+      <c r="D21" s="89"/>
+      <c r="E21" s="89"/>
+      <c r="F21" s="88"/>
+      <c r="H21" s="64"/>
+      <c r="I21" s="64"/>
+      <c r="J21" s="60"/>
+      <c r="K21" s="60"/>
+    </row>
+    <row r="22" spans="2:21" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="40"/>
+      <c r="C22" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="80"/>
+      <c r="E22" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="F22" s="39"/>
+      <c r="H22" s="90" t="s">
+        <v>41</v>
+      </c>
+      <c r="I22" s="91"/>
+      <c r="J22" s="91"/>
+    </row>
+    <row r="23" spans="2:21" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="E23" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="F23" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="H23" s="91"/>
+      <c r="I23" s="91"/>
+      <c r="J23" s="91"/>
+      <c r="K23" s="59"/>
+    </row>
+    <row r="24" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B24" s="18">
+        <v>0</v>
+      </c>
+      <c r="C24" s="20">
+        <v>0</v>
+      </c>
+      <c r="D24" s="19">
+        <v>0</v>
+      </c>
+      <c r="E24" s="34">
+        <v>0</v>
+      </c>
+      <c r="F24" s="30">
+        <v>0</v>
+      </c>
+      <c r="H24" s="57"/>
+      <c r="I24" s="58"/>
+      <c r="J24" s="58"/>
+      <c r="K24" s="58"/>
+      <c r="L24" t="s">
+        <v>6</v>
+      </c>
+      <c r="N24" s="57">
+        <v>1</v>
+      </c>
+      <c r="O24" s="57">
+        <v>1</v>
+      </c>
+      <c r="P24" s="57">
+        <v>1</v>
+      </c>
+      <c r="Q24" s="57">
+        <v>1</v>
+      </c>
+      <c r="R24" s="57">
+        <v>0</v>
+      </c>
+      <c r="S24" s="57">
+        <v>0</v>
+      </c>
+      <c r="T24" s="57">
+        <v>0</v>
+      </c>
+      <c r="U24" s="57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B25" s="29">
+        <v>0</v>
+      </c>
+      <c r="C25" s="21">
+        <v>0</v>
+      </c>
+      <c r="D25" s="19">
+        <v>1</v>
+      </c>
+      <c r="E25" s="17">
+        <v>1</v>
+      </c>
+      <c r="F25" s="30">
+        <v>0</v>
+      </c>
+      <c r="H25" s="57"/>
+      <c r="I25" s="49"/>
+      <c r="J25" s="49"/>
+      <c r="K25" s="49"/>
+      <c r="L25" t="s">
+        <v>7</v>
+      </c>
+      <c r="N25" s="57">
+        <v>1</v>
+      </c>
+      <c r="O25" s="57">
+        <v>1</v>
+      </c>
+      <c r="P25" s="57">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="57">
+        <v>0</v>
+      </c>
+      <c r="R25" s="57">
+        <v>1</v>
+      </c>
+      <c r="S25" s="57">
+        <v>1</v>
+      </c>
+      <c r="T25" s="57">
+        <v>0</v>
+      </c>
+      <c r="U25" s="57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B26" s="29">
+        <v>0</v>
+      </c>
+      <c r="C26" s="21">
+        <v>1</v>
+      </c>
+      <c r="D26" s="19">
+        <v>0</v>
+      </c>
+      <c r="E26" s="17">
+        <v>1</v>
+      </c>
+      <c r="F26" s="30">
+        <v>0</v>
+      </c>
+      <c r="H26" s="57"/>
+      <c r="I26" s="49"/>
+      <c r="J26" s="49"/>
+      <c r="K26" s="49"/>
+      <c r="L26" t="s">
+        <v>21</v>
+      </c>
+      <c r="N26" s="92">
+        <v>1</v>
+      </c>
+      <c r="O26" s="72">
+        <v>0</v>
+      </c>
+      <c r="P26" s="72">
+        <v>1</v>
+      </c>
+      <c r="Q26" s="72">
+        <v>0</v>
+      </c>
+      <c r="R26" s="72">
+        <v>1</v>
+      </c>
+      <c r="S26" s="72">
+        <v>0</v>
+      </c>
+      <c r="T26" s="72">
+        <v>1</v>
+      </c>
+      <c r="U26" s="72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B27" s="18">
+        <v>0</v>
+      </c>
+      <c r="C27" s="15">
+        <v>1</v>
+      </c>
+      <c r="D27" s="19">
+        <v>1</v>
+      </c>
+      <c r="E27" s="21">
+        <v>0</v>
+      </c>
+      <c r="F27" s="35">
+        <v>1</v>
+      </c>
+      <c r="H27" s="57"/>
+      <c r="I27" s="49"/>
+      <c r="J27" s="49"/>
+      <c r="L27" s="61" t="s">
+        <v>35</v>
+      </c>
+      <c r="N27" s="63"/>
+      <c r="O27" s="63"/>
+      <c r="P27" s="63"/>
+      <c r="Q27" s="63"/>
+      <c r="R27" s="63"/>
+      <c r="S27" s="63"/>
+      <c r="T27" s="63"/>
+      <c r="U27" s="63"/>
+    </row>
+    <row r="28" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B28" s="18">
+        <v>1</v>
+      </c>
+      <c r="C28" s="15">
+        <v>0</v>
+      </c>
+      <c r="D28" s="19">
+        <v>0</v>
+      </c>
+      <c r="E28" s="17">
+        <v>1</v>
+      </c>
+      <c r="F28" s="30">
+        <v>0</v>
+      </c>
+      <c r="L28" t="s">
+        <v>22</v>
+      </c>
+      <c r="M28" s="62"/>
+      <c r="N28" s="70">
+        <v>1</v>
+      </c>
+      <c r="O28" s="70">
+        <v>1</v>
+      </c>
+      <c r="P28" s="70">
+        <v>1</v>
+      </c>
+      <c r="Q28" s="70">
+        <v>0</v>
+      </c>
+      <c r="R28" s="70">
+        <v>0</v>
+      </c>
+      <c r="S28" s="70">
+        <v>1</v>
+      </c>
+      <c r="T28" s="70">
+        <v>1</v>
+      </c>
+      <c r="U28" s="70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B29" s="18">
+        <v>1</v>
+      </c>
+      <c r="C29" s="15">
+        <v>0</v>
+      </c>
+      <c r="D29" s="19">
+        <v>1</v>
+      </c>
+      <c r="E29" s="21">
+        <v>0</v>
+      </c>
+      <c r="F29" s="35">
+        <v>1</v>
+      </c>
+      <c r="L29" t="s">
+        <v>23</v>
+      </c>
+      <c r="M29" s="93">
+        <v>1</v>
+      </c>
+      <c r="N29" s="93">
+        <v>1</v>
+      </c>
+      <c r="O29" s="93">
+        <v>1</v>
+      </c>
+      <c r="P29" s="93">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="93">
+        <v>1</v>
+      </c>
+      <c r="R29" s="93">
+        <v>0</v>
+      </c>
+      <c r="S29" s="93">
+        <v>0</v>
+      </c>
+      <c r="T29" s="94">
+        <v>0</v>
+      </c>
+      <c r="U29" s="68"/>
+    </row>
+    <row r="30" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B30" s="18">
+        <v>1</v>
+      </c>
+      <c r="C30" s="15">
+        <v>1</v>
+      </c>
+      <c r="D30" s="19">
+        <v>0</v>
+      </c>
+      <c r="E30" s="21">
+        <v>0</v>
+      </c>
+      <c r="F30" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:21" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="1">
+        <v>1</v>
+      </c>
+      <c r="C31" s="13">
+        <v>1</v>
+      </c>
+      <c r="D31" s="31">
+        <v>1</v>
+      </c>
+      <c r="E31" s="23">
+        <v>1</v>
+      </c>
+      <c r="F31" s="36">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="L3:T3"/>
+    <mergeCell ref="H22:J23"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD13989A-4B85-4E5C-BF76-B025997BE6AB}">
   <dimension ref="B2:C10"/>
   <sheetViews>

</xml_diff>